<commit_message>
Updated Type of activity
</commit_message>
<xml_diff>
--- a/TOUR TO SINGMAL_WBS-With-Gantt-Chart.xlsx
+++ b/TOUR TO SINGMAL_WBS-With-Gantt-Chart.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="242">
   <si>
     <t>TASK OWNER</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>09:00:00 AM to 8 pm</t>
+  </si>
+  <si>
+    <t>Theon Hou - Temple</t>
   </si>
 </sst>
 </file>
@@ -758,9 +761,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="2"/>
@@ -1261,299 +1271,299 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="18" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="18" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="18" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="18" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="23" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="23" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="23" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="23" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="18" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="18" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="18" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="26" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="26" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1562,149 +1572,152 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="29" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="29" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="18" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="18" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="18" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="18" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1762,7 +1775,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDFC03F7-6F07-0948-860A-CE8009F277A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FDFC03F7-6F07-0948-860A-CE8009F277A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1972,7 +1985,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Headlines" id="{3841520A-25F2-4EB8-BE4C-611DB5ABEED9}" vid="{ECD25A4C-D97E-4C12-84B1-63580BFFAEEB}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Headlines" id="{3841520A-25F2-4EB8-BE4C-611DB5ABEED9}" vid="{ECD25A4C-D97E-4C12-84B1-63580BFFAEEB}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4619,45 +4632,45 @@
     </row>
     <row r="34" spans="2:68" ht="10.15" customHeight="1"/>
     <row r="35" spans="2:68" ht="49.9" customHeight="1">
-      <c r="B35" s="131" t="s">
+      <c r="B35" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="132"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="132"/>
-      <c r="F35" s="132"/>
-      <c r="G35" s="132"/>
-      <c r="H35" s="132"/>
-      <c r="I35" s="132"/>
-      <c r="J35" s="132"/>
-      <c r="K35" s="132"/>
-      <c r="L35" s="132"/>
-      <c r="M35" s="132"/>
-      <c r="N35" s="132"/>
-      <c r="O35" s="132"/>
-      <c r="P35" s="132"/>
-      <c r="Q35" s="132"/>
-      <c r="R35" s="132"/>
-      <c r="S35" s="132"/>
-      <c r="T35" s="132"/>
-      <c r="U35" s="132"/>
-      <c r="V35" s="132"/>
-      <c r="W35" s="132"/>
-      <c r="X35" s="132"/>
-      <c r="Y35" s="132"/>
-      <c r="Z35" s="132"/>
-      <c r="AA35" s="132"/>
-      <c r="AB35" s="132"/>
-      <c r="AC35" s="132"/>
-      <c r="AD35" s="132"/>
-      <c r="AE35" s="132"/>
-      <c r="AF35" s="132"/>
-      <c r="AG35" s="132"/>
-      <c r="AH35" s="132"/>
-      <c r="AI35" s="132"/>
-      <c r="AJ35" s="132"/>
-      <c r="AK35" s="132"/>
-      <c r="AL35" s="132"/>
+      <c r="C35" s="137"/>
+      <c r="D35" s="137"/>
+      <c r="E35" s="137"/>
+      <c r="F35" s="137"/>
+      <c r="G35" s="137"/>
+      <c r="H35" s="137"/>
+      <c r="I35" s="137"/>
+      <c r="J35" s="137"/>
+      <c r="K35" s="137"/>
+      <c r="L35" s="137"/>
+      <c r="M35" s="137"/>
+      <c r="N35" s="137"/>
+      <c r="O35" s="137"/>
+      <c r="P35" s="137"/>
+      <c r="Q35" s="137"/>
+      <c r="R35" s="137"/>
+      <c r="S35" s="137"/>
+      <c r="T35" s="137"/>
+      <c r="U35" s="137"/>
+      <c r="V35" s="137"/>
+      <c r="W35" s="137"/>
+      <c r="X35" s="137"/>
+      <c r="Y35" s="137"/>
+      <c r="Z35" s="137"/>
+      <c r="AA35" s="137"/>
+      <c r="AB35" s="137"/>
+      <c r="AC35" s="137"/>
+      <c r="AD35" s="137"/>
+      <c r="AE35" s="137"/>
+      <c r="AF35" s="137"/>
+      <c r="AG35" s="137"/>
+      <c r="AH35" s="137"/>
+      <c r="AI35" s="137"/>
+      <c r="AJ35" s="137"/>
+      <c r="AK35" s="137"/>
+      <c r="AL35" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5122,24 +5135,24 @@
       <c r="AJ7" s="68"/>
       <c r="AK7" s="68"/>
       <c r="AL7" s="68"/>
-      <c r="AM7" s="133" t="s">
+      <c r="AM7" s="138" t="s">
         <v>96</v>
       </c>
-      <c r="AN7" s="133"/>
-      <c r="AO7" s="133"/>
-      <c r="AP7" s="133"/>
-      <c r="AQ7" s="133"/>
-      <c r="AR7" s="133"/>
-      <c r="AS7" s="133"/>
-      <c r="AT7" s="133" t="s">
+      <c r="AN7" s="138"/>
+      <c r="AO7" s="138"/>
+      <c r="AP7" s="138"/>
+      <c r="AQ7" s="138"/>
+      <c r="AR7" s="138"/>
+      <c r="AS7" s="138"/>
+      <c r="AT7" s="138" t="s">
         <v>97</v>
       </c>
-      <c r="AU7" s="133"/>
-      <c r="AV7" s="133"/>
-      <c r="AW7" s="133"/>
-      <c r="AX7" s="133"/>
-      <c r="AY7" s="133"/>
-      <c r="AZ7" s="133"/>
+      <c r="AU7" s="138"/>
+      <c r="AV7" s="138"/>
+      <c r="AW7" s="138"/>
+      <c r="AX7" s="138"/>
+      <c r="AY7" s="138"/>
+      <c r="AZ7" s="138"/>
       <c r="BD7" s="110">
         <v>43645</v>
       </c>
@@ -8778,7 +8791,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9608,8 +9621,8 @@
         <v>193</v>
       </c>
       <c r="C33" s="90"/>
-      <c r="D33" s="88" t="s">
-        <v>194</v>
+      <c r="D33" s="149" t="s">
+        <v>241</v>
       </c>
       <c r="E33" s="88" t="s">
         <v>195</v>
@@ -9625,28 +9638,28 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="148" customFormat="1">
-      <c r="A34" s="144" t="s">
+    <row r="34" spans="1:8" s="135" customFormat="1">
+      <c r="A34" s="131" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="145" t="s">
+      <c r="B34" s="132" t="s">
         <v>193</v>
       </c>
-      <c r="C34" s="146"/>
-      <c r="D34" s="145" t="s">
+      <c r="C34" s="133"/>
+      <c r="D34" s="132" t="s">
         <v>239</v>
       </c>
-      <c r="E34" s="144" t="s">
+      <c r="E34" s="131" t="s">
         <v>240</v>
       </c>
-      <c r="F34" s="144">
+      <c r="F34" s="131">
         <v>2884</v>
       </c>
-      <c r="G34" s="144">
+      <c r="G34" s="131">
         <f t="shared" si="1"/>
         <v>5768</v>
       </c>
-      <c r="H34" s="147"/>
+      <c r="H34" s="134"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9677,25 +9690,25 @@
       <c r="B2" s="108" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="146" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="143"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="148"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="108" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="137" t="s">
+      <c r="C3" s="142" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="138"/>
-      <c r="E3" s="139" t="s">
+      <c r="D3" s="143"/>
+      <c r="E3" s="144" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="140"/>
+      <c r="F3" s="145"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="108" t="s">
@@ -9715,7 +9728,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="40.5">
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="139" t="s">
         <v>209</v>
       </c>
       <c r="C5" s="103" t="s">
@@ -9732,7 +9745,7 @@
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="135"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="103" t="s">
         <v>102</v>
       </c>
@@ -9747,7 +9760,7 @@
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="135"/>
+      <c r="B7" s="140"/>
       <c r="C7" s="103" t="s">
         <v>85</v>
       </c>
@@ -9762,7 +9775,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="27">
-      <c r="B8" s="135"/>
+      <c r="B8" s="140"/>
       <c r="C8" s="103" t="s">
         <v>81</v>
       </c>
@@ -9777,7 +9790,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" ht="27">
-      <c r="B9" s="135"/>
+      <c r="B9" s="140"/>
       <c r="C9" s="103" t="s">
         <v>87</v>
       </c>
@@ -9792,7 +9805,7 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="135"/>
+      <c r="B10" s="140"/>
       <c r="C10" s="103" t="s">
         <v>120</v>
       </c>
@@ -9807,7 +9820,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" ht="40.5">
-      <c r="B11" s="135"/>
+      <c r="B11" s="140"/>
       <c r="C11" s="103" t="s">
         <v>121</v>
       </c>
@@ -9822,7 +9835,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" ht="30">
-      <c r="B12" s="135"/>
+      <c r="B12" s="140"/>
       <c r="C12" s="103" t="s">
         <v>124</v>
       </c>
@@ -9837,7 +9850,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="27">
-      <c r="B13" s="135"/>
+      <c r="B13" s="140"/>
       <c r="C13" s="103" t="s">
         <v>125</v>
       </c>
@@ -9852,7 +9865,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="27">
-      <c r="B14" s="135"/>
+      <c r="B14" s="140"/>
       <c r="C14" s="103" t="s">
         <v>142</v>
       </c>
@@ -9867,7 +9880,7 @@
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="135"/>
+      <c r="B15" s="140"/>
       <c r="C15" s="102"/>
       <c r="D15" s="104" t="s">
         <v>132</v>
@@ -9878,7 +9891,7 @@
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="135"/>
+      <c r="B16" s="140"/>
       <c r="C16" s="102"/>
       <c r="D16" s="105" t="s">
         <v>134</v>
@@ -9889,7 +9902,7 @@
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="135"/>
+      <c r="B17" s="140"/>
       <c r="C17" s="102"/>
       <c r="D17" s="105" t="s">
         <v>158</v>
@@ -9900,7 +9913,7 @@
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="135"/>
+      <c r="B18" s="140"/>
       <c r="C18" s="102"/>
       <c r="D18" s="105" t="s">
         <v>159</v>
@@ -9911,7 +9924,7 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="135"/>
+      <c r="B19" s="140"/>
       <c r="C19" s="102"/>
       <c r="D19" s="105" t="s">
         <v>160</v>
@@ -9920,7 +9933,7 @@
       <c r="F19" s="99"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="135"/>
+      <c r="B20" s="140"/>
       <c r="C20" s="102"/>
       <c r="D20" s="105" t="s">
         <v>174</v>
@@ -9929,7 +9942,7 @@
       <c r="F20" s="99"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="136"/>
+      <c r="B21" s="141"/>
       <c r="C21" s="102"/>
       <c r="D21" s="105" t="s">
         <v>175</v>

</xml_diff>